<commit_message>
Improve export test files.
</commit_message>
<xml_diff>
--- a/emr/exports/templates/export-template-list.test.xlsx
+++ b/emr/exports/templates/export-template-list.test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="23540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="(Config)" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="63">
   <si>
     <t>Sheet Num</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>Reason for absence</t>
+  </si>
+  <si>
+    <t>(empty)</t>
+  </si>
+  <si>
+    <t>not slug</t>
   </si>
 </sst>
 </file>
@@ -212,15 +218,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -260,8 +267,14 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF963634"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +287,18 @@
         <bgColor rgb="FFCCDDFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DCDB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -284,7 +309,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -297,8 +322,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -311,27 +354,50 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="heading" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -720,9 +786,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:M6"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -731,7 +799,7 @@
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
@@ -741,7 +809,201 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:13" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:15" ht="15" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
@@ -754,7 +1016,9 @@
       <c r="F5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
@@ -773,40 +1037,156 @@
       <c r="M5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="3:13" ht="15" customHeight="1">
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="N5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1">
+      <c r="A6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="11" t="s">
         <v>22</v>
+      </c>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1">
+      <c r="A7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1">
+      <c r="A10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +1202,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -833,21 +1213,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="44.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="44.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -855,32 +1234,91 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1">
+      <c r="A2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -895,7 +1333,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -918,13 +1356,14 @@
     <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:22" s="5" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -968,72 +1407,184 @@
         <v>51</v>
       </c>
       <c r="O1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="T1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" s="12" t="s">
         <v>59</v>
+      </c>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>